<commit_message>
코드 정리 및 WidgetManager 생성
</commit_message>
<xml_diff>
--- a/GameData/BlindStat.xlsx
+++ b/GameData/BlindStat.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>SMALL</t>
+    <t>SMallGrade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Round</t>
+    <t>BigGrade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BIG</t>
+    <t>BossGrade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BOSS</t>
+    <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -85,12 +85,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,7 +412,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -420,21 +423,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
@@ -449,9 +449,6 @@
       <c r="D2" s="1">
         <v>600</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
@@ -466,9 +463,6 @@
       <c r="D3" s="1">
         <v>1600</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
@@ -483,9 +477,6 @@
       <c r="D4" s="1">
         <v>4000</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
@@ -500,9 +491,6 @@
       <c r="D5" s="1">
         <v>10000</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
@@ -517,9 +505,6 @@
       <c r="D6" s="1">
         <v>19000</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
@@ -534,9 +519,6 @@
       <c r="D7" s="1">
         <v>38000</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
@@ -551,9 +533,6 @@
       <c r="D8" s="1">
         <v>65000</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
@@ -568,9 +547,6 @@
       <c r="D9" s="1">
         <v>130000</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10"/>
@@ -604,7 +580,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>

</xml_diff>